<commit_message>
Updates Charts Authantication Session
Authentication has been added
</commit_message>
<xml_diff>
--- a/customer.xlsx
+++ b/customer.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="93">
   <si>
     <t>Id</t>
   </si>
@@ -242,6 +242,54 @@
   </si>
   <si>
     <t>denemekullanici1234</t>
+  </si>
+  <si>
+    <t>Binbaşı (Kara Kuvvetleri)</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Genel Müdür Yardımcısı-Eğitim, Sağlık, Spor (</t>
+  </si>
+  <si>
+    <t>Muhtar-Köy</t>
+  </si>
+  <si>
+    <t>Binbaşı (Jandarma)</t>
+  </si>
+  <si>
+    <t>gathaus</t>
+  </si>
+  <si>
+    <t>Albay (Sahil Güvenlik)</t>
+  </si>
+  <si>
+    <t>Genel Müdür-Eğitim, Sağlık, Spor (Özel Sektör</t>
+  </si>
+  <si>
+    <t>(Lisans Programı 4-6 Yıllık)ıştay Başkanı</t>
+  </si>
+  <si>
+    <t>Yönetici-Elektrik, Havagazı, Su Ve Sıhhi Tesi</t>
+  </si>
+  <si>
+    <t>Ayakkabı ve Saraciye Teknolojisi Öğretmeni</t>
+  </si>
+  <si>
+    <t>Genel Müdür-İnşaat Ve İmalat Sanayi (Özel Sek</t>
+  </si>
+  <si>
+    <t>Genel Müdür-Bankalar Ve Mali Müesseseler (Öze</t>
+  </si>
+  <si>
+    <t>Halk Oyunları Oyuncusu (Siirt Yöresi)</t>
+  </si>
+  <si>
+    <t>Genel Müdür Yardımcısı-Bankalar Ve Mali Müess</t>
+  </si>
+  <si>
+    <t>Genel Müdür Yardımcısı-İnşaat Ve İmalat Sanay</t>
   </si>
 </sst>
 </file>
@@ -618,7 +666,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I65"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -1990,6 +2038,528 @@
         <v>14</v>
       </c>
     </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" t="s">
+        <v>77</v>
+      </c>
+      <c r="I48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49" t="s">
+        <v>79</v>
+      </c>
+      <c r="I49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" t="s">
+        <v>75</v>
+      </c>
+      <c r="H50" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" t="s">
+        <v>75</v>
+      </c>
+      <c r="H51" t="s">
+        <v>81</v>
+      </c>
+      <c r="I51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+      <c r="F52" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53">
+        <v>22</v>
+      </c>
+      <c r="D53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" t="s">
+        <v>84</v>
+      </c>
+      <c r="I53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54">
+        <v>22</v>
+      </c>
+      <c r="D54" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" t="s">
+        <v>85</v>
+      </c>
+      <c r="I54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55">
+        <v>22</v>
+      </c>
+      <c r="D55" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" t="s">
+        <v>34</v>
+      </c>
+      <c r="G55" t="s">
+        <v>39</v>
+      </c>
+      <c r="H55" t="s">
+        <v>86</v>
+      </c>
+      <c r="I55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56">
+        <v>22</v>
+      </c>
+      <c r="D56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" t="s">
+        <v>34</v>
+      </c>
+      <c r="G56" t="s">
+        <v>75</v>
+      </c>
+      <c r="H56" t="s">
+        <v>87</v>
+      </c>
+      <c r="I56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57">
+        <v>22</v>
+      </c>
+      <c r="D57" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" t="s">
+        <v>39</v>
+      </c>
+      <c r="H57" t="s">
+        <v>88</v>
+      </c>
+      <c r="I57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58">
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>29</v>
+      </c>
+      <c r="E58" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G58" t="s">
+        <v>75</v>
+      </c>
+      <c r="H58" t="s">
+        <v>89</v>
+      </c>
+      <c r="I58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59">
+        <v>22</v>
+      </c>
+      <c r="D59" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F59" t="s">
+        <v>34</v>
+      </c>
+      <c r="G59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H59" t="s">
+        <v>90</v>
+      </c>
+      <c r="I59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60">
+        <v>22</v>
+      </c>
+      <c r="D60" t="s">
+        <v>29</v>
+      </c>
+      <c r="E60" t="s">
+        <v>34</v>
+      </c>
+      <c r="F60" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" t="s">
+        <v>75</v>
+      </c>
+      <c r="H60" t="s">
+        <v>89</v>
+      </c>
+      <c r="I60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61">
+        <v>22</v>
+      </c>
+      <c r="D61" t="s">
+        <v>29</v>
+      </c>
+      <c r="E61" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" t="s">
+        <v>34</v>
+      </c>
+      <c r="G61" t="s">
+        <v>39</v>
+      </c>
+      <c r="H61" t="s">
+        <v>86</v>
+      </c>
+      <c r="I61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" t="s">
+        <v>34</v>
+      </c>
+      <c r="G62" t="s">
+        <v>75</v>
+      </c>
+      <c r="H62" t="s">
+        <v>88</v>
+      </c>
+      <c r="I62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63">
+        <v>22</v>
+      </c>
+      <c r="D63" t="s">
+        <v>29</v>
+      </c>
+      <c r="E63" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" t="s">
+        <v>34</v>
+      </c>
+      <c r="G63" t="s">
+        <v>75</v>
+      </c>
+      <c r="H63" t="s">
+        <v>91</v>
+      </c>
+      <c r="I63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64">
+        <v>22</v>
+      </c>
+      <c r="D64" t="s">
+        <v>29</v>
+      </c>
+      <c r="E64" t="s">
+        <v>34</v>
+      </c>
+      <c r="F64" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" t="s">
+        <v>39</v>
+      </c>
+      <c r="H64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65">
+        <v>22</v>
+      </c>
+      <c r="D65" t="s">
+        <v>29</v>
+      </c>
+      <c r="E65" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" t="s">
+        <v>34</v>
+      </c>
+      <c r="G65" t="s">
+        <v>75</v>
+      </c>
+      <c r="H65" t="s">
+        <v>88</v>
+      </c>
+      <c r="I65" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>